<commit_message>
minor template updates in inst/extdata
</commit_message>
<xml_diff>
--- a/inst/extdata/MassWateR_DQOAccuracy_Template.xlsx
+++ b/inst/extdata/MassWateR_DQOAccuracy_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d8cbaaa4eaa566d/Documents/1 ACASAK/MassWateR/Design/Templates for users/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557988E-4E29-4824-A2B2-C842145FABF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{8557988E-4E29-4824-A2B2-C842145FABF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA8FB4E1-AD4F-4AD6-8A1B-2E1312F763CB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="168">
   <si>
     <t>Parameter</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Upper Quantitation Limit.  If the Result Value is AQL and no value is entered in the Results file Quantitation Limit column, then this value will be used.  Enter "na" if there is no limit.  MassWateR analytical functions will use 100% of the UQL for data purposes.</t>
   </si>
   <si>
-    <t>Template updated 8/16/23</t>
-  </si>
-  <si>
     <t>Minimum Detection Level.  If the Result Value is BDL and no value is entered in the Results file Quantitation Limit column, then this value will be used.  Enter "na" if there is no minimum.  MassWateR analytical functions will use 1/2 of the MDL for data purposes.</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>deg F</t>
   </si>
   <si>
-    <t>Cyanobacteria (lab)</t>
-  </si>
-  <si>
     <t>FAU</t>
   </si>
   <si>
@@ -528,6 +522,24 @@
   </si>
   <si>
     <t>Water Temp</t>
+  </si>
+  <si>
+    <t>RFU</t>
+  </si>
+  <si>
+    <t>Template updated 10/28/24</t>
+  </si>
+  <si>
+    <t>Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Phycocyanin</t>
+  </si>
+  <si>
+    <t>Phycocyanin (probe)</t>
+  </si>
+  <si>
+    <t>Phycoerythrin</t>
   </si>
 </sst>
 </file>
@@ -806,9 +818,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -846,7 +858,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -952,7 +964,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1094,7 +1106,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1108,7 +1120,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,17 +1457,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E51C4DBB-7A06-4B01-9EB2-015D10941B0A}">
+          <x14:formula1>
+            <xm:f>Values!$B$2:$B$43</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4EA15E2-D832-4A49-BBD2-136FE3197BAC}">
           <x14:formula1>
-            <xm:f>Values!$A$2:$A$65</xm:f>
+            <xm:f>Values!$A$2:$A$68</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E51C4DBB-7A06-4B01-9EB2-015D10941B0A}">
-          <x14:formula1>
-            <xm:f>Values!$B$2:$B$42</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1471,7 +1483,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1499,7 @@
         <v>48</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>64</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1547,7 +1559,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="13">
         <v>0.1</v>
@@ -1676,11 +1688,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618763B1-9045-410C-ABE3-5B174AA86A7D}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,63 +1711,63 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
         <v>72</v>
-      </c>
-      <c r="B4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
         <v>74</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
         <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
         <v>78</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
         <v>80</v>
-      </c>
-      <c r="B8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -1763,74 +1775,74 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
         <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
         <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1838,15 +1850,15 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1854,36 +1866,36 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
@@ -1891,82 +1903,82 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,170 +1986,188 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>163</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>